<commit_message>
Avoided double entry for skill id in candidate skill table
</commit_message>
<xml_diff>
--- a/NLP/File-validation/Book1.xlsx
+++ b/NLP/File-validation/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python-Projects\NLP\File-validation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{400077CA-253D-4E36-A84E-F5BDBA53DDED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{847ED013-6D1A-4AEB-8B79-A74FB8482FD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CE2BFC06-1CD4-4BA5-A1DF-2FB367F7E886}"/>
   </bookViews>
@@ -79,9 +79,6 @@
     <t>skill2 years</t>
   </si>
   <si>
-    <t>skill 3</t>
-  </si>
-  <si>
     <t>skill3 years</t>
   </si>
   <si>
@@ -164,6 +161,9 @@
   </si>
   <si>
     <t>15-13-2000</t>
+  </si>
+  <si>
+    <t>skill3</t>
   </si>
 </sst>
 </file>
@@ -530,7 +530,7 @@
   <dimension ref="A1:O12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="Q8" sqref="Q8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -593,21 +593,21 @@
         <v>12</v>
       </c>
       <c r="N1" t="s">
+        <v>41</v>
+      </c>
+      <c r="O1" t="s">
         <v>13</v>
-      </c>
-      <c r="O1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B2">
         <v>1234567890</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D2" s="2">
         <v>44873.395833333336</v>
@@ -616,7 +616,7 @@
         <v>55</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G2">
         <v>2</v>
@@ -628,13 +628,13 @@
         <v>7.5</v>
       </c>
       <c r="J2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K2">
         <v>1</v>
       </c>
       <c r="L2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M2">
         <v>2</v>
@@ -642,13 +642,13 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B3">
         <v>2345678901</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D3" s="2">
         <v>44874.395833333336</v>
@@ -657,7 +657,7 @@
         <v>66</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G3">
         <v>3</v>
@@ -669,19 +669,19 @@
         <v>9</v>
       </c>
       <c r="J3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K3">
         <v>2</v>
       </c>
       <c r="L3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="M3">
         <v>1</v>
       </c>
       <c r="N3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="O3">
         <v>1</v>
@@ -689,7 +689,7 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B4">
         <v>3456789912</v>
@@ -708,19 +708,19 @@
         <v>8</v>
       </c>
       <c r="J4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K4">
         <v>3</v>
       </c>
       <c r="L4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M4">
         <v>2</v>
       </c>
       <c r="N4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="O4">
         <v>5</v>
@@ -731,7 +731,7 @@
         <v>4567900923</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D5" s="2">
         <v>44876.395833333336</v>
@@ -740,7 +740,7 @@
         <v>88</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G5">
         <v>3</v>
@@ -752,19 +752,19 @@
         <v>12</v>
       </c>
       <c r="J5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K5">
         <v>2</v>
       </c>
       <c r="L5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="M5">
         <v>5</v>
       </c>
       <c r="N5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="O5">
         <v>4</v>
@@ -772,20 +772,20 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B6">
         <v>5679011934</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6">
         <v>99</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G6">
         <v>2</v>
@@ -797,19 +797,19 @@
         <v>13.5</v>
       </c>
       <c r="J6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K6">
         <v>6</v>
       </c>
       <c r="L6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M6">
         <v>4</v>
       </c>
       <c r="N6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="O6">
         <v>2</v>
@@ -820,7 +820,7 @@
         <v>6790122945</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D7" s="2">
         <v>44878.395833333336</v>
@@ -829,25 +829,25 @@
         <v>110</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I7">
         <v>15</v>
       </c>
       <c r="J7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K7">
         <v>5</v>
       </c>
       <c r="L7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="M7">
         <v>3</v>
       </c>
       <c r="N7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="O7">
         <v>8</v>
@@ -855,7 +855,7 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D8" s="2">
         <v>44879.395833333336</v>
@@ -864,7 +864,7 @@
         <v>121</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G8">
         <v>3</v>
@@ -876,13 +876,13 @@
         <v>16.5</v>
       </c>
       <c r="L8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M8">
         <v>6</v>
       </c>
       <c r="N8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="O8">
         <v>7</v>
@@ -890,16 +890,16 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B9">
         <v>901234490</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E9">
         <v>132</v>
@@ -915,13 +915,13 @@
         <v>18</v>
       </c>
       <c r="J9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K9">
         <v>3</v>
       </c>
       <c r="L9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="M9">
         <v>8</v>
@@ -929,7 +929,7 @@
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="C10" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D10" s="2">
         <v>44881.395833333336</v>
@@ -938,7 +938,7 @@
         <v>143</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G10">
         <v>1</v>
@@ -950,19 +950,19 @@
         <v>19.5</v>
       </c>
       <c r="J10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K10">
         <v>8</v>
       </c>
       <c r="L10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M10">
         <v>9</v>
       </c>
       <c r="N10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="O10">
         <v>7</v>
@@ -970,13 +970,13 @@
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B11">
         <v>7901233956</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D11" s="2">
         <v>44882.395833333336</v>
@@ -985,7 +985,7 @@
         <v>154</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G11">
         <v>2</v>
@@ -997,13 +997,13 @@
         <v>21</v>
       </c>
       <c r="J11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K11">
         <v>4</v>
       </c>
       <c r="N11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="O11">
         <v>5</v>
@@ -1011,13 +1011,13 @@
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B12">
         <v>1357986420</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D12" s="2">
         <v>44883.395833333336</v>
@@ -1026,7 +1026,7 @@
         <v>165</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H12">
         <v>20</v>
@@ -1035,19 +1035,19 @@
         <v>22.5</v>
       </c>
       <c r="J12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K12">
         <v>6</v>
       </c>
       <c r="L12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M12">
         <v>7</v>
       </c>
       <c r="N12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="O12">
         <v>4</v>

</xml_diff>